<commit_message>
backtesting de rsi actualizado a abrir hasta 10 operaciones a la vez. Proximo paso: cambiar todos los backtesting
</commit_message>
<xml_diff>
--- a/tick.xlsx
+++ b/tick.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B292"/>
+  <dimension ref="A1:B277"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,2911 +448,2761 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2023-02-01</t>
+          <t>2023-03-01</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>171.78</v>
+        <v>28.555</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2023-02-02</t>
+          <t>2023-03-02</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>186.77</v>
+        <v>28.903</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2023-02-03</t>
+          <t>2023-03-03</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>189.41</v>
+        <v>28.628</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2023-02-06</t>
+          <t>2023-03-06</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>196.65</v>
+        <v>28.762</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2023-02-07</t>
+          <t>2023-03-07</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>195.12</v>
+        <v>28.633</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2023-02-08</t>
+          <t>2023-03-08</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>195.52</v>
+        <v>28.876</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2023-02-09</t>
+          <t>2023-03-09</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>207.45</v>
+        <v>28.762</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2023-02-10</t>
+          <t>2023-03-10</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>204.06</v>
+        <v>28.054</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2023-02-13</t>
+          <t>2023-03-13</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>191.02</v>
+        <v>28.23</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2023-02-14</t>
+          <t>2023-03-14</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>193.52</v>
+        <v>28.176</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2023-02-15</t>
+          <t>2023-03-15</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>212.33</v>
+        <v>28.844</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2023-02-16</t>
+          <t>2023-03-16</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>210.45</v>
+        <v>28.43</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2023-02-17</t>
+          <t>2023-03-17</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>204.25</v>
+        <v>28.603</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2023-02-21</t>
+          <t>2023-03-20</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>206.07</v>
+        <v>28.173</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2023-02-22</t>
+          <t>2023-03-21</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>197.7</v>
+        <v>28.736</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2023-02-23</t>
+          <t>2023-03-22</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>204.95</v>
+        <v>29.052</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2023-02-24</t>
+          <t>2023-03-23</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>196.98</v>
+        <v>28.982</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2023-02-27</t>
+          <t>2023-03-24</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>203.8</v>
+        <v>28.587</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2023-02-28</t>
+          <t>2023-03-27</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>208.94</v>
+        <v>28.204</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2023-03-01</t>
+          <t>2023-03-28</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>204.24</v>
+        <v>28.326</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2023-03-02</t>
+          <t>2023-03-29</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>189.03</v>
+        <v>28.296</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2023-03-03</t>
+          <t>2023-03-30</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>194.06</v>
+        <v>28.962</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2023-03-06</t>
+          <t>2023-03-31</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>196.65</v>
+        <v>29.292</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2023-03-07</t>
+          <t>2023-04-03</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>191.88</v>
+        <v>29.225</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2023-03-08</t>
+          <t>2023-04-04</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>183.66</v>
+        <v>29.485</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2023-03-09</t>
+          <t>2023-04-05</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>182.4</v>
+        <v>29.578</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2023-03-10</t>
+          <t>2023-04-06</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>172.78</v>
+        <v>29.495</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2023-03-13</t>
+          <t>2023-04-11</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>166.99</v>
+        <v>29.722</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2023-03-14</t>
+          <t>2023-04-12</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>180.96</v>
+        <v>29.414</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2023-03-15</t>
+          <t>2023-04-13</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>180.25</v>
+        <v>29.964</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2023-03-16</t>
+          <t>2023-04-14</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>179.5</v>
+        <v>30.237</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2023-03-17</t>
+          <t>2023-04-17</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>184</v>
+        <v>30.704</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2023-03-20</t>
+          <t>2023-04-18</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>177.25</v>
+        <v>30.978</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2023-03-21</t>
+          <t>2023-04-19</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>189.01</v>
+        <v>31.113</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2023-03-22</t>
+          <t>2023-04-20</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>198.75</v>
+        <v>31.402</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2023-03-23</t>
+          <t>2023-04-21</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>197.58</v>
+        <v>31.393</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2023-03-24</t>
+          <t>2023-04-24</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>190.7</v>
+        <v>31.729</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2023-03-27</t>
+          <t>2023-04-25</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>196.29</v>
+        <v>31.558</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2023-03-28</t>
+          <t>2023-04-26</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>190.71</v>
+        <v>31.388</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2023-03-29</t>
+          <t>2023-04-27</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>194.25</v>
+        <v>31.266</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2023-03-30</t>
+          <t>2023-04-28</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>195.95</v>
+        <v>31.209</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2023-03-31</t>
+          <t>2023-05-02</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>197.96</v>
+        <v>31.202</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2023-04-03</t>
+          <t>2023-05-03</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>202.56</v>
+        <v>31.163</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2023-04-04</t>
+          <t>2023-05-04</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>198.43</v>
+        <v>31.379</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2023-04-05</t>
+          <t>2023-05-05</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>189.84</v>
+        <v>31.537</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2023-04-06</t>
+          <t>2023-05-08</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>180.43</v>
+        <v>31.609</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2023-04-10</t>
+          <t>2023-05-09</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>177.43</v>
+        <v>31.772</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2023-04-11</t>
+          <t>2023-05-10</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>187.76</v>
+        <v>31.956</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2023-04-12</t>
+          <t>2023-05-11</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>189.75</v>
+        <v>32.054</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2023-04-13</t>
+          <t>2023-05-12</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>182.41</v>
+        <v>31.874</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2023-04-14</t>
+          <t>2023-05-15</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>182.85</v>
+        <v>31.097</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2023-04-17</t>
+          <t>2023-05-16</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>185.94</v>
+        <v>30.867</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2023-04-18</t>
+          <t>2023-05-17</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>186.92</v>
+        <v>30.917</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2023-04-19</t>
+          <t>2023-05-18</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>179.32</v>
+        <v>31.19</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2023-04-20</t>
+          <t>2023-05-19</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>167.29</v>
+        <v>31.232</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2023-04-21</t>
+          <t>2023-05-22</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>162.67</v>
+        <v>31.433</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2023-04-24</t>
+          <t>2023-05-23</t>
         </is>
       </c>
       <c r="B58" t="n">
-        <v>163.55</v>
+        <v>31.309</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2023-04-25</t>
+          <t>2023-05-24</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>159.35</v>
+        <v>30.887</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2023-04-26</t>
+          <t>2023-05-25</t>
         </is>
       </c>
       <c r="B60" t="n">
-        <v>159.49</v>
+        <v>30.8</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2023-04-27</t>
+          <t>2023-05-26</t>
         </is>
       </c>
       <c r="B61" t="n">
-        <v>154.29</v>
+        <v>31.023</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2023-04-28</t>
+          <t>2023-05-29</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>158.33</v>
+        <v>31.397</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2023-05-01</t>
+          <t>2023-05-30</t>
         </is>
       </c>
       <c r="B63" t="n">
-        <v>161.4</v>
+        <v>31.147</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2023-05-02</t>
+          <t>2023-05-31</t>
         </is>
       </c>
       <c r="B64" t="n">
-        <v>164.32</v>
+        <v>30.967</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>2023-05-03</t>
+          <t>2023-06-01</t>
         </is>
       </c>
       <c r="B65" t="n">
-        <v>161.56</v>
+        <v>31.458</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>2023-05-04</t>
+          <t>2023-06-02</t>
         </is>
       </c>
       <c r="B66" t="n">
-        <v>162.07</v>
+        <v>31.579</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>2023-05-05</t>
+          <t>2023-06-05</t>
         </is>
       </c>
       <c r="B67" t="n">
-        <v>165.06</v>
+        <v>31.318</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>2023-05-08</t>
+          <t>2023-06-06</t>
         </is>
       </c>
       <c r="B68" t="n">
-        <v>171.05</v>
+        <v>31.33</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>2023-05-09</t>
+          <t>2023-06-07</t>
         </is>
       </c>
       <c r="B69" t="n">
-        <v>169.18</v>
+        <v>31.209</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>2023-05-10</t>
+          <t>2023-06-08</t>
         </is>
       </c>
       <c r="B70" t="n">
-        <v>173.42</v>
+        <v>31.168</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>2023-05-11</t>
+          <t>2023-06-09</t>
         </is>
       </c>
       <c r="B71" t="n">
-        <v>167.47</v>
+        <v>31.364</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>2023-05-12</t>
+          <t>2023-06-12</t>
         </is>
       </c>
       <c r="B72" t="n">
-        <v>176.02</v>
+        <v>31.555</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>2023-05-15</t>
+          <t>2023-06-13</t>
         </is>
       </c>
       <c r="B73" t="n">
-        <v>168.76</v>
+        <v>31.956</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>2023-05-16</t>
+          <t>2023-06-14</t>
         </is>
       </c>
       <c r="B74" t="n">
-        <v>166.55</v>
+        <v>31.404</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>2023-05-17</t>
+          <t>2023-06-15</t>
         </is>
       </c>
       <c r="B75" t="n">
-        <v>167.43</v>
+        <v>31.113</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>2023-05-18</t>
+          <t>2023-06-16</t>
         </is>
       </c>
       <c r="B76" t="n">
-        <v>174.13</v>
+        <v>31.391</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>2023-05-19</t>
+          <t>2023-06-19</t>
         </is>
       </c>
       <c r="B77" t="n">
-        <v>178.23</v>
+        <v>31.479</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>2023-05-22</t>
+          <t>2023-06-20</t>
         </is>
       </c>
       <c r="B78" t="n">
-        <v>182.85</v>
+        <v>31.107</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>2023-05-23</t>
+          <t>2023-06-21</t>
         </is>
       </c>
       <c r="B79" t="n">
-        <v>187.85</v>
+        <v>31.149</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>2023-05-24</t>
+          <t>2023-06-22</t>
         </is>
       </c>
       <c r="B80" t="n">
-        <v>182.76</v>
+        <v>30.991</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>2023-05-25</t>
+          <t>2023-06-23</t>
         </is>
       </c>
       <c r="B81" t="n">
-        <v>185.22</v>
+        <v>31.001</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>2023-05-26</t>
+          <t>2023-06-26</t>
         </is>
       </c>
       <c r="B82" t="n">
-        <v>186.83</v>
+        <v>31</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>2023-05-30</t>
+          <t>2023-06-27</t>
         </is>
       </c>
       <c r="B83" t="n">
-        <v>201.96</v>
+        <v>31.211</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>2023-05-31</t>
+          <t>2023-06-28</t>
         </is>
       </c>
       <c r="B84" t="n">
-        <v>199.19</v>
+        <v>31.43</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>2023-06-01</t>
+          <t>2023-06-29</t>
         </is>
       </c>
       <c r="B85" t="n">
-        <v>202.02</v>
+        <v>31.521</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>2023-06-02</t>
+          <t>2023-06-30</t>
         </is>
       </c>
       <c r="B86" t="n">
-        <v>212.14</v>
+        <v>31.883</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>2023-06-05</t>
+          <t>2023-07-03</t>
         </is>
       </c>
       <c r="B87" t="n">
-        <v>220.89</v>
+        <v>32.086</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>2023-06-06</t>
+          <t>2023-07-04</t>
         </is>
       </c>
       <c r="B88" t="n">
-        <v>214.5</v>
+        <v>30.308</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>2023-06-07</t>
+          <t>2023-07-05</t>
         </is>
       </c>
       <c r="B89" t="n">
-        <v>228.38</v>
+        <v>30.055</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>2023-06-08</t>
+          <t>2023-07-06</t>
         </is>
       </c>
       <c r="B90" t="n">
-        <v>224.89</v>
+        <v>29.642</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>2023-06-09</t>
+          <t>2023-07-07</t>
         </is>
       </c>
       <c r="B91" t="n">
-        <v>248.74</v>
+        <v>29.153</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>2023-06-12</t>
+          <t>2023-07-10</t>
         </is>
       </c>
       <c r="B92" t="n">
-        <v>248.82</v>
+        <v>29.389</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>2023-06-13</t>
+          <t>2023-07-11</t>
         </is>
       </c>
       <c r="B93" t="n">
-        <v>255.33</v>
+        <v>29.691</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>2023-06-14</t>
+          <t>2023-07-12</t>
         </is>
       </c>
       <c r="B94" t="n">
-        <v>258.03</v>
+        <v>30.126</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>2023-06-15</t>
+          <t>2023-07-13</t>
         </is>
       </c>
       <c r="B95" t="n">
-        <v>251.79</v>
+        <v>29.84</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>2023-06-16</t>
+          <t>2023-07-14</t>
         </is>
       </c>
       <c r="B96" t="n">
-        <v>259.47</v>
+        <v>30.098</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>2023-06-20</t>
+          <t>2023-07-17</t>
         </is>
       </c>
       <c r="B97" t="n">
-        <v>264.43</v>
+        <v>29.759</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>2023-06-21</t>
+          <t>2023-07-18</t>
         </is>
       </c>
       <c r="B98" t="n">
-        <v>275.17</v>
+        <v>29.782</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>2023-06-22</t>
+          <t>2023-07-19</t>
         </is>
       </c>
       <c r="B99" t="n">
-        <v>254.32</v>
+        <v>30.129</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>2023-06-23</t>
+          <t>2023-07-20</t>
         </is>
       </c>
       <c r="B100" t="n">
-        <v>260.99</v>
+        <v>30.524</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>2023-06-26</t>
+          <t>2023-07-21</t>
         </is>
       </c>
       <c r="B101" t="n">
-        <v>254.3</v>
+        <v>30.844</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>2023-06-27</t>
+          <t>2023-07-24</t>
         </is>
       </c>
       <c r="B102" t="n">
-        <v>243.34</v>
+        <v>30.443</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>2023-06-28</t>
+          <t>2023-07-25</t>
         </is>
       </c>
       <c r="B103" t="n">
-        <v>251.05</v>
+        <v>30.435</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>2023-06-29</t>
+          <t>2023-07-26</t>
         </is>
       </c>
       <c r="B104" t="n">
-        <v>260.69</v>
+        <v>30.618</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>2023-06-30</t>
+          <t>2023-07-27</t>
         </is>
       </c>
       <c r="B105" t="n">
-        <v>261</v>
+        <v>31.72</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>2023-07-03</t>
+          <t>2023-07-28</t>
         </is>
       </c>
       <c r="B106" t="n">
-        <v>278.74</v>
+        <v>31.937</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>2023-07-05</t>
+          <t>2023-07-31</t>
         </is>
       </c>
       <c r="B107" t="n">
-        <v>278.81</v>
+        <v>31.881</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>2023-07-06</t>
+          <t>2023-08-01</t>
         </is>
       </c>
       <c r="B108" t="n">
-        <v>278.3</v>
+        <v>31.816</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>2023-07-07</t>
+          <t>2023-08-02</t>
         </is>
       </c>
       <c r="B109" t="n">
-        <v>279.21</v>
+        <v>31.292</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>2023-07-10</t>
+          <t>2023-08-03</t>
         </is>
       </c>
       <c r="B110" t="n">
-        <v>274.47</v>
+        <v>31.445</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>2023-07-11</t>
+          <t>2023-08-04</t>
         </is>
       </c>
       <c r="B111" t="n">
-        <v>269.4</v>
+        <v>31.253</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>2023-07-12</t>
+          <t>2023-08-07</t>
         </is>
       </c>
       <c r="B112" t="n">
-        <v>274.39</v>
+        <v>31.298</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>2023-07-13</t>
+          <t>2023-08-08</t>
         </is>
       </c>
       <c r="B113" t="n">
-        <v>273.89</v>
+        <v>31.397</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>2023-07-14</t>
+          <t>2023-08-09</t>
         </is>
       </c>
       <c r="B114" t="n">
-        <v>278.21</v>
+        <v>31.574</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>2023-07-17</t>
+          <t>2023-08-10</t>
         </is>
       </c>
       <c r="B115" t="n">
-        <v>290.19</v>
+        <v>31.734</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>2023-07-18</t>
+          <t>2023-08-11</t>
         </is>
       </c>
       <c r="B116" t="n">
-        <v>287.59</v>
+        <v>31.843</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>2023-07-19</t>
+          <t>2023-08-14</t>
         </is>
       </c>
       <c r="B117" t="n">
-        <v>295.22</v>
+        <v>31.663</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>2023-07-20</t>
+          <t>2023-08-15</t>
         </is>
       </c>
       <c r="B118" t="n">
-        <v>280.31</v>
+        <v>31.767</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>2023-07-21</t>
+          <t>2023-08-16</t>
         </is>
       </c>
       <c r="B119" t="n">
-        <v>264.12</v>
+        <v>31.545</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>2023-07-24</t>
+          <t>2023-08-17</t>
         </is>
       </c>
       <c r="B120" t="n">
-        <v>257.2</v>
+        <v>31.38</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>2023-07-25</t>
+          <t>2023-08-18</t>
         </is>
       </c>
       <c r="B121" t="n">
-        <v>270.29</v>
+        <v>31.17</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>2023-07-26</t>
+          <t>2023-08-21</t>
         </is>
       </c>
       <c r="B122" t="n">
-        <v>261.9</v>
+        <v>31.495</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>2023-07-27</t>
+          <t>2023-08-22</t>
         </is>
       </c>
       <c r="B123" t="n">
-        <v>268.06</v>
+        <v>31.489</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>2023-07-28</t>
+          <t>2023-08-23</t>
         </is>
       </c>
       <c r="B124" t="n">
-        <v>258.82</v>
+        <v>31.777</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>2023-07-31</t>
+          <t>2023-08-24</t>
         </is>
       </c>
       <c r="B125" t="n">
-        <v>267.09</v>
+        <v>31.964</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>2023-08-01</t>
+          <t>2023-08-25</t>
         </is>
       </c>
       <c r="B126" t="n">
-        <v>264.22</v>
+        <v>31.934</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>2023-08-02</t>
+          <t>2023-08-28</t>
         </is>
       </c>
       <c r="B127" t="n">
-        <v>255.13</v>
+        <v>32.04</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>2023-08-03</t>
+          <t>2023-08-29</t>
         </is>
       </c>
       <c r="B128" t="n">
-        <v>253.5</v>
+        <v>32.276</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>2023-08-04</t>
+          <t>2023-08-30</t>
         </is>
       </c>
       <c r="B129" t="n">
-        <v>263.09</v>
+        <v>32.333</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>2023-08-07</t>
+          <t>2023-08-31</t>
         </is>
       </c>
       <c r="B130" t="n">
-        <v>251.9</v>
+        <v>32.505</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>2023-08-08</t>
+          <t>2023-09-01</t>
         </is>
       </c>
       <c r="B131" t="n">
-        <v>248.61</v>
+        <v>32.36</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>2023-08-09</t>
+          <t>2023-09-04</t>
         </is>
       </c>
       <c r="B132" t="n">
-        <v>248.35</v>
+        <v>32.498</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>2023-08-10</t>
+          <t>2023-09-05</t>
         </is>
       </c>
       <c r="B133" t="n">
-        <v>246.16</v>
+        <v>32.234</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>2023-08-11</t>
+          <t>2023-09-06</t>
         </is>
       </c>
       <c r="B134" t="n">
-        <v>241.4</v>
+        <v>32.235</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>2023-08-14</t>
+          <t>2023-09-07</t>
         </is>
       </c>
       <c r="B135" t="n">
-        <v>234.92</v>
+        <v>32.147</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>2023-08-15</t>
+          <t>2023-09-08</t>
         </is>
       </c>
       <c r="B136" t="n">
-        <v>239.28</v>
+        <v>32.627</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>2023-08-16</t>
+          <t>2023-09-11</t>
         </is>
       </c>
       <c r="B137" t="n">
-        <v>229.68</v>
+        <v>32.688</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>2023-08-17</t>
+          <t>2023-09-12</t>
         </is>
       </c>
       <c r="B138" t="n">
-        <v>224.07</v>
+        <v>32.999</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>2023-08-18</t>
+          <t>2023-09-13</t>
         </is>
       </c>
       <c r="B139" t="n">
-        <v>216.55</v>
+        <v>32.731</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>2023-08-21</t>
+          <t>2023-09-14</t>
         </is>
       </c>
       <c r="B140" t="n">
-        <v>221.72</v>
+        <v>32.661</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>2023-08-22</t>
+          <t>2023-09-15</t>
         </is>
       </c>
       <c r="B141" t="n">
-        <v>239.32</v>
+        <v>33.081</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>2023-08-23</t>
+          <t>2023-09-18</t>
         </is>
       </c>
       <c r="B142" t="n">
-        <v>231.07</v>
+        <v>33.442</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>2023-08-24</t>
+          <t>2023-09-19</t>
         </is>
       </c>
       <c r="B143" t="n">
-        <v>235.46</v>
+        <v>33.517</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>2023-08-25</t>
+          <t>2023-09-20</t>
         </is>
       </c>
       <c r="B144" t="n">
-        <v>233.56</v>
+        <v>34.323</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>2023-08-28</t>
+          <t>2023-09-21</t>
         </is>
       </c>
       <c r="B145" t="n">
-        <v>241.87</v>
+        <v>34.215</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>2023-08-29</t>
+          <t>2023-09-22</t>
         </is>
       </c>
       <c r="B146" t="n">
-        <v>240.29</v>
+        <v>33.814</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>2023-08-30</t>
+          <t>2023-09-25</t>
         </is>
       </c>
       <c r="B147" t="n">
-        <v>254.63</v>
+        <v>33.976</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>2023-08-31</t>
+          <t>2023-09-26</t>
         </is>
       </c>
       <c r="B148" t="n">
-        <v>257.29</v>
+        <v>33.879</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>2023-09-01</t>
+          <t>2023-09-27</t>
         </is>
       </c>
       <c r="B149" t="n">
-        <v>256.44</v>
+        <v>33.898</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>2023-09-05</t>
+          <t>2023-09-28</t>
         </is>
       </c>
       <c r="B150" t="n">
-        <v>248.48</v>
+        <v>33.889</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>2023-09-06</t>
+          <t>2023-09-29</t>
         </is>
       </c>
       <c r="B151" t="n">
-        <v>252.29</v>
+        <v>33.914</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>2023-09-07</t>
+          <t>2023-10-02</t>
         </is>
       </c>
       <c r="B152" t="n">
-        <v>244.04</v>
+        <v>34.2</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>2023-09-08</t>
+          <t>2023-10-03</t>
         </is>
       </c>
       <c r="B153" t="n">
-        <v>255.61</v>
+        <v>33.541</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>2023-09-11</t>
+          <t>2023-10-04</t>
         </is>
       </c>
       <c r="B154" t="n">
-        <v>261.78</v>
+        <v>33.239</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>2023-09-12</t>
+          <t>2023-10-05</t>
         </is>
       </c>
       <c r="B155" t="n">
-        <v>269.59</v>
+        <v>33.106</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>2023-09-13</t>
+          <t>2023-10-06</t>
         </is>
       </c>
       <c r="B156" t="n">
-        <v>271.86</v>
+        <v>32.128</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>2023-09-14</t>
+          <t>2023-10-09</t>
         </is>
       </c>
       <c r="B157" t="n">
-        <v>271.22</v>
+        <v>33.085</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>2023-09-15</t>
+          <t>2023-10-10</t>
         </is>
       </c>
       <c r="B158" t="n">
-        <v>276.41</v>
+        <v>33.362</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>2023-09-18</t>
+          <t>2023-10-11</t>
         </is>
       </c>
       <c r="B159" t="n">
-        <v>268.99</v>
+        <v>33.316</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>2023-09-19</t>
+          <t>2023-10-12</t>
         </is>
       </c>
       <c r="B160" t="n">
-        <v>267.56</v>
+        <v>33.675</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>2023-09-20</t>
+          <t>2023-10-13</t>
         </is>
       </c>
       <c r="B161" t="n">
-        <v>266.14</v>
+        <v>33.7</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>2023-09-21</t>
+          <t>2023-10-16</t>
         </is>
       </c>
       <c r="B162" t="n">
-        <v>258.3</v>
+        <v>33.409</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>2023-09-22</t>
+          <t>2023-10-17</t>
         </is>
       </c>
       <c r="B163" t="n">
-        <v>255.9</v>
+        <v>33.038</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>2023-09-25</t>
+          <t>2023-10-18</t>
         </is>
       </c>
       <c r="B164" t="n">
-        <v>238.89</v>
+        <v>33.104</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>2023-09-26</t>
+          <t>2023-10-19</t>
         </is>
       </c>
       <c r="B165" t="n">
-        <v>244.78</v>
+        <v>32.619</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>2023-09-27</t>
+          <t>2023-10-20</t>
         </is>
       </c>
       <c r="B166" t="n">
-        <v>242.85</v>
+        <v>32.528</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>2023-09-28</t>
+          <t>2023-10-23</t>
         </is>
       </c>
       <c r="B167" t="n">
-        <v>241.59</v>
+        <v>32.325</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>2023-09-29</t>
+          <t>2023-10-24</t>
         </is>
       </c>
       <c r="B168" t="n">
-        <v>251.76</v>
+        <v>32.359</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>2023-10-02</t>
+          <t>2023-10-25</t>
         </is>
       </c>
       <c r="B169" t="n">
-        <v>243.5</v>
+        <v>32.623</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>2023-10-03</t>
+          <t>2023-10-26</t>
         </is>
       </c>
       <c r="B170" t="n">
-        <v>247.41</v>
+        <v>32.348</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>2023-10-04</t>
+          <t>2023-10-27</t>
         </is>
       </c>
       <c r="B171" t="n">
-        <v>250.22</v>
+        <v>32.939</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>2023-10-05</t>
+          <t>2023-10-30</t>
         </is>
       </c>
       <c r="B172" t="n">
-        <v>262.94</v>
+        <v>33.825</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>2023-10-06</t>
+          <t>2023-10-31</t>
         </is>
       </c>
       <c r="B173" t="n">
-        <v>253.94</v>
+        <v>33.78</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>2023-10-09</t>
+          <t>2023-11-01</t>
         </is>
       </c>
       <c r="B174" t="n">
-        <v>254.36</v>
+        <v>34.161</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>2023-10-10</t>
+          <t>2023-11-02</t>
         </is>
       </c>
       <c r="B175" t="n">
-        <v>260.66</v>
+        <v>34.402</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>2023-10-11</t>
+          <t>2023-11-03</t>
         </is>
       </c>
       <c r="B176" t="n">
-        <v>268.21</v>
+        <v>34.392</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>2023-10-12</t>
+          <t>2023-11-06</t>
         </is>
       </c>
       <c r="B177" t="n">
-        <v>264.45</v>
+        <v>33.737</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>2023-10-13</t>
+          <t>2023-11-07</t>
         </is>
       </c>
       <c r="B178" t="n">
-        <v>257.23</v>
+        <v>33.239</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>2023-10-16</t>
+          <t>2023-11-08</t>
         </is>
       </c>
       <c r="B179" t="n">
-        <v>253.52</v>
+        <v>33.027</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>2023-10-17</t>
+          <t>2023-11-09</t>
         </is>
       </c>
       <c r="B180" t="n">
-        <v>249.39</v>
+        <v>33.218</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>2023-10-18</t>
+          <t>2023-11-10</t>
         </is>
       </c>
       <c r="B181" t="n">
-        <v>254.55</v>
+        <v>33.362</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>2023-10-19</t>
+          <t>2023-11-13</t>
         </is>
       </c>
       <c r="B182" t="n">
-        <v>228.39</v>
+        <v>33.48</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>2023-10-20</t>
+          <t>2023-11-14</t>
         </is>
       </c>
       <c r="B183" t="n">
-        <v>214.7</v>
+        <v>33.928</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>2023-10-23</t>
+          <t>2023-11-15</t>
         </is>
       </c>
       <c r="B184" t="n">
-        <v>206.36</v>
+        <v>34.502</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>2023-10-24</t>
+          <t>2023-11-16</t>
         </is>
       </c>
       <c r="B185" t="n">
-        <v>218.03</v>
+        <v>35.048</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>2023-10-25</t>
+          <t>2023-11-17</t>
         </is>
       </c>
       <c r="B186" t="n">
-        <v>215.17</v>
+        <v>35.653</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>2023-10-26</t>
+          <t>2023-11-20</t>
         </is>
       </c>
       <c r="B187" t="n">
-        <v>212.51</v>
+        <v>35.875</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>2023-10-27</t>
+          <t>2023-11-21</t>
         </is>
       </c>
       <c r="B188" t="n">
-        <v>211.12</v>
+        <v>35.978</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>2023-10-30</t>
+          <t>2023-11-22</t>
         </is>
       </c>
       <c r="B189" t="n">
-        <v>209.85</v>
+        <v>36.099</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>2023-10-31</t>
+          <t>2023-11-23</t>
         </is>
       </c>
       <c r="B190" t="n">
-        <v>196.58</v>
+        <v>35.98</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>2023-11-01</t>
+          <t>2023-11-24</t>
         </is>
       </c>
       <c r="B191" t="n">
-        <v>202.01</v>
+        <v>36.01</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>2023-11-02</t>
+          <t>2023-11-27</t>
         </is>
       </c>
       <c r="B192" t="n">
-        <v>211.85</v>
+        <v>36.242</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>2023-11-03</t>
+          <t>2023-11-28</t>
         </is>
       </c>
       <c r="B193" t="n">
-        <v>221.21</v>
+        <v>36.561</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>2023-11-06</t>
+          <t>2023-11-29</t>
         </is>
       </c>
       <c r="B194" t="n">
-        <v>223.36</v>
+        <v>36.63</v>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>2023-11-07</t>
+          <t>2023-11-30</t>
         </is>
       </c>
       <c r="B195" t="n">
-        <v>218.18</v>
+        <v>36.657</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>2023-11-08</t>
+          <t>2023-12-01</t>
         </is>
       </c>
       <c r="B196" t="n">
-        <v>221.42</v>
+        <v>36.951</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>2023-11-09</t>
+          <t>2023-12-04</t>
         </is>
       </c>
       <c r="B197" t="n">
-        <v>218.39</v>
+        <v>37.008</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>2023-11-10</t>
+          <t>2023-12-05</t>
         </is>
       </c>
       <c r="B198" t="n">
-        <v>210.73</v>
+        <v>36.974</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>2023-11-13</t>
+          <t>2023-12-06</t>
         </is>
       </c>
       <c r="B199" t="n">
-        <v>214.16</v>
+        <v>37.215</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>2023-11-14</t>
+          <t>2023-12-07</t>
         </is>
       </c>
       <c r="B200" t="n">
-        <v>231.74</v>
+        <v>36.998</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>2023-11-15</t>
+          <t>2023-12-08</t>
         </is>
       </c>
       <c r="B201" t="n">
-        <v>239.98</v>
+        <v>37.179</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>2023-11-16</t>
+          <t>2023-12-11</t>
         </is>
       </c>
       <c r="B202" t="n">
-        <v>239.79</v>
+        <v>37.55</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>2023-11-17</t>
+          <t>2023-12-12</t>
         </is>
       </c>
       <c r="B203" t="n">
-        <v>229.21</v>
+        <v>37.774</v>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>2023-11-20</t>
+          <t>2023-12-13</t>
         </is>
       </c>
       <c r="B204" t="n">
-        <v>231.4</v>
+        <v>38.299</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>2023-11-21</t>
+          <t>2023-12-14</t>
         </is>
       </c>
       <c r="B205" t="n">
-        <v>236.9</v>
+        <v>39.57</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>2023-11-22</t>
+          <t>2023-12-15</t>
         </is>
       </c>
       <c r="B206" t="n">
-        <v>241.47</v>
+        <v>39.796</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>2023-11-24</t>
+          <t>2023-12-18</t>
         </is>
       </c>
       <c r="B207" t="n">
-        <v>236.05</v>
+        <v>39.432</v>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>2023-11-27</t>
+          <t>2023-12-19</t>
         </is>
       </c>
       <c r="B208" t="n">
-        <v>233.31</v>
+        <v>39.38</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>2023-11-28</t>
+          <t>2023-12-20</t>
         </is>
       </c>
       <c r="B209" t="n">
-        <v>237.58</v>
+        <v>39.624</v>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>2023-11-29</t>
+          <t>2023-12-21</t>
         </is>
       </c>
       <c r="B210" t="n">
-        <v>251.98</v>
+        <v>39.452</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>2023-11-30</t>
+          <t>2023-12-22</t>
         </is>
       </c>
       <c r="B211" t="n">
-        <v>242.57</v>
+        <v>39.935</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>2023-12-01</t>
+          <t>2023-12-27</t>
         </is>
       </c>
       <c r="B212" t="n">
-        <v>232.67</v>
+        <v>39.766</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>2023-12-04</t>
+          <t>2023-12-28</t>
         </is>
       </c>
       <c r="B213" t="n">
-        <v>236.85</v>
+        <v>40.127</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>2023-12-05</t>
+          <t>2023-12-29</t>
         </is>
       </c>
       <c r="B214" t="n">
-        <v>236.82</v>
+        <v>40.231</v>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>2023-12-06</t>
+          <t>2024-01-02</t>
         </is>
       </c>
       <c r="B215" t="n">
-        <v>243.76</v>
+        <v>40.639</v>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>2023-12-07</t>
+          <t>2024-01-03</t>
         </is>
       </c>
       <c r="B216" t="n">
-        <v>240.78</v>
+        <v>40.227</v>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>2023-12-08</t>
+          <t>2024-01-04</t>
         </is>
       </c>
       <c r="B217" t="n">
-        <v>241.23</v>
+        <v>39.661</v>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>2023-12-11</t>
+          <t>2024-01-05</t>
         </is>
       </c>
       <c r="B218" t="n">
-        <v>241.51</v>
+        <v>39.634</v>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>2023-12-12</t>
+          <t>2024-01-08</t>
         </is>
       </c>
       <c r="B219" t="n">
-        <v>235.23</v>
+        <v>39.68</v>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>2023-12-13</t>
+          <t>2024-01-09</t>
         </is>
       </c>
       <c r="B220" t="n">
-        <v>236.69</v>
+        <v>39.656</v>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>2023-12-14</t>
+          <t>2024-01-10</t>
         </is>
       </c>
       <c r="B221" t="n">
-        <v>243.77</v>
+        <v>39.377</v>
       </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>2023-12-15</t>
+          <t>2024-01-11</t>
         </is>
       </c>
       <c r="B222" t="n">
-        <v>250.74</v>
+        <v>39.521</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>2023-12-18</t>
+          <t>2024-01-12</t>
         </is>
       </c>
       <c r="B223" t="n">
-        <v>255.79</v>
+        <v>40.068</v>
       </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>2023-12-19</t>
+          <t>2024-01-15</t>
         </is>
       </c>
       <c r="B224" t="n">
-        <v>255.14</v>
+        <v>40.28</v>
       </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>2023-12-20</t>
+          <t>2024-01-16</t>
         </is>
       </c>
       <c r="B225" t="n">
-        <v>255.61</v>
+        <v>39.927</v>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>2023-12-21</t>
+          <t>2024-01-17</t>
         </is>
       </c>
       <c r="B226" t="n">
-        <v>253.72</v>
+        <v>39.337</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>2023-12-22</t>
+          <t>2024-01-18</t>
         </is>
       </c>
       <c r="B227" t="n">
-        <v>256.69</v>
+        <v>39.614</v>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>2023-12-26</t>
+          <t>2024-01-19</t>
         </is>
       </c>
       <c r="B228" t="n">
-        <v>254.16</v>
+        <v>39.326</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>2023-12-27</t>
+          <t>2024-01-22</t>
         </is>
       </c>
       <c r="B229" t="n">
-        <v>260.22</v>
+        <v>39.589</v>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>2023-12-28</t>
+          <t>2024-01-23</t>
         </is>
       </c>
       <c r="B230" t="n">
-        <v>263.67</v>
+        <v>39.817</v>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>2023-12-29</t>
+          <t>2024-01-24</t>
         </is>
       </c>
       <c r="B231" t="n">
-        <v>252.56</v>
+        <v>39.46</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>2024-01-02</t>
+          <t>2024-01-25</t>
         </is>
       </c>
       <c r="B232" t="n">
-        <v>245.11</v>
+        <v>39.446</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>2024-01-03</t>
+          <t>2024-01-26</t>
         </is>
       </c>
       <c r="B233" t="n">
-        <v>241.49</v>
+        <v>39.43</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>2024-01-04</t>
+          <t>2024-01-29</t>
         </is>
       </c>
       <c r="B234" t="n">
-        <v>240.89</v>
+        <v>39.608</v>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>2024-01-05</t>
+          <t>2024-01-30</t>
         </is>
       </c>
       <c r="B235" t="n">
-        <v>236.69</v>
+        <v>35.818</v>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>2024-01-08</t>
+          <t>2024-01-31</t>
         </is>
       </c>
       <c r="B236" t="n">
-        <v>237.55</v>
+        <v>36.382</v>
       </c>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>2024-01-09</t>
+          <t>2024-02-01</t>
         </is>
       </c>
       <c r="B237" t="n">
-        <v>238</v>
+        <v>36.639</v>
       </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>2024-01-10</t>
+          <t>2024-02-02</t>
         </is>
       </c>
       <c r="B238" t="n">
-        <v>233.48</v>
+        <v>36.827</v>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>2024-01-11</t>
+          <t>2024-02-05</t>
         </is>
       </c>
       <c r="B239" t="n">
-        <v>228.88</v>
+        <v>37.041</v>
       </c>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>2024-01-12</t>
+          <t>2024-02-06</t>
         </is>
       </c>
       <c r="B240" t="n">
-        <v>223.55</v>
+        <v>36.959</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>2024-01-16</t>
+          <t>2024-02-07</t>
         </is>
       </c>
       <c r="B241" t="n">
-        <v>212.32</v>
+        <v>36.629</v>
       </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>2024-01-17</t>
+          <t>2024-02-08</t>
         </is>
       </c>
       <c r="B242" t="n">
-        <v>212.71</v>
+        <v>36.161</v>
       </c>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>2024-01-18</t>
+          <t>2024-02-09</t>
         </is>
       </c>
       <c r="B243" t="n">
-        <v>215.78</v>
+        <v>36.177</v>
       </c>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>2024-01-19</t>
+          <t>2024-02-12</t>
         </is>
       </c>
       <c r="B244" t="n">
-        <v>211.89</v>
+        <v>36.139</v>
       </c>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>2024-01-22</t>
+          <t>2024-02-13</t>
         </is>
       </c>
       <c r="B245" t="n">
-        <v>214.25</v>
+        <v>36.239</v>
       </c>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>2024-01-23</t>
+          <t>2024-02-14</t>
         </is>
       </c>
       <c r="B246" t="n">
-        <v>212.46</v>
+        <v>36.473</v>
       </c>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>2024-01-24</t>
+          <t>2024-02-15</t>
         </is>
       </c>
       <c r="B247" t="n">
-        <v>211.13</v>
+        <v>36.978</v>
       </c>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>2024-01-25</t>
+          <t>2024-02-16</t>
         </is>
       </c>
       <c r="B248" t="n">
-        <v>189.5</v>
+        <v>37.187</v>
       </c>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>2024-01-26</t>
+          <t>2024-02-19</t>
         </is>
       </c>
       <c r="B249" t="n">
-        <v>185.16</v>
+        <v>36.496</v>
       </c>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>2024-01-29</t>
+          <t>2024-02-20</t>
         </is>
       </c>
       <c r="B250" t="n">
-        <v>185.53</v>
+        <v>36.736</v>
       </c>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>2024-01-30</t>
+          <t>2024-02-21</t>
         </is>
       </c>
       <c r="B251" t="n">
-        <v>193.98</v>
+        <v>36.698</v>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>2024-01-31</t>
+          <t>2024-02-22</t>
         </is>
       </c>
       <c r="B252" t="n">
-        <v>188.91</v>
+        <v>37.225</v>
       </c>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>2024-02-01</t>
+          <t>2024-02-23</t>
         </is>
       </c>
       <c r="B253" t="n">
-        <v>188.6</v>
+        <v>37.158</v>
       </c>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>2024-02-02</t>
+          <t>2024-02-26</t>
         </is>
       </c>
       <c r="B254" t="n">
-        <v>185.31</v>
+        <v>37.092</v>
       </c>
     </row>
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>2024-02-05</t>
+          <t>2024-02-27</t>
         </is>
       </c>
       <c r="B255" t="n">
-        <v>183.96</v>
+        <v>37</v>
       </c>
     </row>
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>2024-02-06</t>
+          <t>2024-02-28</t>
         </is>
       </c>
       <c r="B256" t="n">
-        <v>181.04</v>
+        <v>37.634</v>
       </c>
     </row>
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>2024-02-07</t>
+          <t>2024-02-29</t>
         </is>
       </c>
       <c r="B257" t="n">
-        <v>187.6</v>
+        <v>37.597</v>
       </c>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>2024-02-08</t>
+          <t>2024-03-01</t>
         </is>
       </c>
       <c r="B258" t="n">
-        <v>186.95</v>
+        <v>36.691</v>
       </c>
     </row>
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>2024-02-09</t>
+          <t>2024-03-04</t>
         </is>
       </c>
       <c r="B259" t="n">
-        <v>191.91</v>
+        <v>37.126</v>
       </c>
     </row>
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>2024-02-12</t>
+          <t>2024-03-05</t>
         </is>
       </c>
       <c r="B260" t="n">
-        <v>193.33</v>
+        <v>37.836</v>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>2024-02-13</t>
+          <t>2024-03-06</t>
         </is>
       </c>
       <c r="B261" t="n">
-        <v>185.06</v>
+        <v>37.954</v>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>2024-02-14</t>
+          <t>2024-03-07</t>
         </is>
       </c>
       <c r="B262" t="n">
-        <v>186.54</v>
+        <v>38.859</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>2024-02-15</t>
+          <t>2024-03-08</t>
         </is>
       </c>
       <c r="B263" t="n">
-        <v>192.76</v>
+        <v>39.375</v>
       </c>
     </row>
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>2024-02-16</t>
+          <t>2024-03-11</t>
         </is>
       </c>
       <c r="B264" t="n">
-        <v>198.83</v>
+        <v>38.92</v>
       </c>
     </row>
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>2024-02-20</t>
+          <t>2024-03-12</t>
         </is>
       </c>
       <c r="B265" t="n">
-        <v>198.39</v>
+        <v>38.945</v>
       </c>
     </row>
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>2024-02-21</t>
+          <t>2024-03-13</t>
         </is>
       </c>
       <c r="B266" t="n">
-        <v>195.83</v>
+        <v>38.982</v>
       </c>
     </row>
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>2024-02-22</t>
+          <t>2024-03-14</t>
         </is>
       </c>
       <c r="B267" t="n">
-        <v>191.95</v>
+        <v>40.147</v>
       </c>
     </row>
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>2024-02-23</t>
+          <t>2024-03-15</t>
         </is>
       </c>
       <c r="B268" t="n">
-        <v>196.92</v>
+        <v>39.752</v>
       </c>
     </row>
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>2024-02-26</t>
+          <t>2024-03-18</t>
         </is>
       </c>
       <c r="B269" t="n">
-        <v>194.58</v>
+        <v>40.173</v>
       </c>
     </row>
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>2024-02-27</t>
+          <t>2024-03-19</t>
         </is>
       </c>
       <c r="B270" t="n">
-        <v>203.52</v>
+        <v>39.403</v>
       </c>
     </row>
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>2024-02-28</t>
+          <t>2024-03-20</t>
         </is>
       </c>
       <c r="B271" t="n">
-        <v>200.23</v>
+        <v>40.109</v>
       </c>
     </row>
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>2024-02-29</t>
+          <t>2024-03-21</t>
         </is>
       </c>
       <c r="B272" t="n">
-        <v>203.67</v>
+        <v>40.502</v>
       </c>
     </row>
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>2024-03-01</t>
+          <t>2024-03-22</t>
         </is>
       </c>
       <c r="B273" t="n">
-        <v>199.94</v>
+        <v>40.643</v>
       </c>
     </row>
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>2024-03-04</t>
+          <t>2024-03-25</t>
         </is>
       </c>
       <c r="B274" t="n">
-        <v>196.35</v>
+        <v>40.539</v>
       </c>
     </row>
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>2024-03-05</t>
+          <t>2024-03-26</t>
         </is>
       </c>
       <c r="B275" t="n">
-        <v>183.53</v>
+        <v>40.282</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>2024-03-06</t>
+          <t>2024-03-27</t>
         </is>
       </c>
       <c r="B276" t="n">
-        <v>179.06</v>
+        <v>40.158</v>
       </c>
     </row>
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>2024-03-07</t>
+          <t>2024-03-28</t>
         </is>
       </c>
       <c r="B277" t="n">
-        <v>178.26</v>
-      </c>
-    </row>
-    <row r="278">
-      <c r="A278" t="inlineStr">
-        <is>
-          <t>2024-03-08</t>
-        </is>
-      </c>
-      <c r="B278" t="n">
-        <v>180.75</v>
-      </c>
-    </row>
-    <row r="279">
-      <c r="A279" t="inlineStr">
-        <is>
-          <t>2024-03-11</t>
-        </is>
-      </c>
-      <c r="B279" t="n">
-        <v>177.05</v>
-      </c>
-    </row>
-    <row r="280">
-      <c r="A280" t="inlineStr">
-        <is>
-          <t>2024-03-12</t>
-        </is>
-      </c>
-      <c r="B280" t="n">
-        <v>175.22</v>
-      </c>
-    </row>
-    <row r="281">
-      <c r="A281" t="inlineStr">
-        <is>
-          <t>2024-03-13</t>
-        </is>
-      </c>
-      <c r="B281" t="n">
-        <v>175.12</v>
-      </c>
-    </row>
-    <row r="282">
-      <c r="A282" t="inlineStr">
-        <is>
-          <t>2024-03-14</t>
-        </is>
-      </c>
-      <c r="B282" t="n">
-        <v>171.17</v>
-      </c>
-    </row>
-    <row r="283">
-      <c r="A283" t="inlineStr">
-        <is>
-          <t>2024-03-15</t>
-        </is>
-      </c>
-      <c r="B283" t="n">
-        <v>164.9</v>
-      </c>
-    </row>
-    <row r="284">
-      <c r="A284" t="inlineStr">
-        <is>
-          <t>2024-03-18</t>
-        </is>
-      </c>
-      <c r="B284" t="n">
-        <v>168.63</v>
-      </c>
-    </row>
-    <row r="285">
-      <c r="A285" t="inlineStr">
-        <is>
-          <t>2024-03-19</t>
-        </is>
-      </c>
-      <c r="B285" t="n">
-        <v>170.65</v>
-      </c>
-    </row>
-    <row r="286">
-      <c r="A286" t="inlineStr">
-        <is>
-          <t>2024-03-20</t>
-        </is>
-      </c>
-      <c r="B286" t="n">
-        <v>174.2</v>
-      </c>
-    </row>
-    <row r="287">
-      <c r="A287" t="inlineStr">
-        <is>
-          <t>2024-03-21</t>
-        </is>
-      </c>
-      <c r="B287" t="n">
-        <v>176.19</v>
-      </c>
-    </row>
-    <row r="288">
-      <c r="A288" t="inlineStr">
-        <is>
-          <t>2024-03-22</t>
-        </is>
-      </c>
-      <c r="B288" t="n">
-        <v>167.89</v>
-      </c>
-    </row>
-    <row r="289">
-      <c r="A289" t="inlineStr">
-        <is>
-          <t>2024-03-25</t>
-        </is>
-      </c>
-      <c r="B289" t="n">
-        <v>174.18</v>
-      </c>
-    </row>
-    <row r="290">
-      <c r="A290" t="inlineStr">
-        <is>
-          <t>2024-03-26</t>
-        </is>
-      </c>
-      <c r="B290" t="n">
-        <v>178.7</v>
-      </c>
-    </row>
-    <row r="291">
-      <c r="A291" t="inlineStr">
-        <is>
-          <t>2024-03-27</t>
-        </is>
-      </c>
-      <c r="B291" t="n">
-        <v>178.85</v>
-      </c>
-    </row>
-    <row r="292">
-      <c r="A292" t="inlineStr">
-        <is>
-          <t>2024-03-28</t>
-        </is>
-      </c>
-      <c r="B292" t="n">
-        <v>179.27</v>
+        <v>38.588</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
funcionando con varios equipos estrategia del futbol
</commit_message>
<xml_diff>
--- a/tick.xlsx
+++ b/tick.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B246"/>
+  <dimension ref="A1:B258"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,2451 +451,2571 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>45022</v>
+        <v>45019</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>22.67</t>
+          <t>212.95</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>45027</v>
+        <v>45020</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>22.40</t>
+          <t>213.20</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>45028</v>
+        <v>45021</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>22.35</t>
+          <t>213.10</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>45029</v>
+        <v>45022</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>22.18</t>
+          <t>216.35</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>45030</v>
+        <v>45027</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>22.21</t>
+          <t>216.40</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>45033</v>
+        <v>45028</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>22.33</t>
+          <t>218.40</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>45034</v>
+        <v>45029</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>22.47</t>
+          <t>219.10</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>45035</v>
+        <v>45030</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>22.44</t>
+          <t>219.10</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>45036</v>
+        <v>45033</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>22.43</t>
+          <t>216.50</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>45037</v>
+        <v>45034</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>22.43</t>
+          <t>219.00</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>45040</v>
+        <v>45035</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>22.09</t>
+          <t>221.75</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>45041</v>
+        <v>45036</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>22.15</t>
+          <t>222.25</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>45042</v>
+        <v>45037</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>22.18</t>
+          <t>222.55</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>45043</v>
+        <v>45040</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>22.22</t>
+          <t>223.75</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>45044</v>
+        <v>45041</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>21.90</t>
+          <t>224.10</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>45048</v>
+        <v>45042</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>21.40</t>
+          <t>223.20</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>45049</v>
+        <v>45043</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>21.21</t>
+          <t>226.25</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>45050</v>
+        <v>45044</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>21.12</t>
+          <t>227.45</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>45051</v>
+        <v>45048</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>21.36</t>
+          <t>222.35</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>45054</v>
+        <v>45049</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>21.23</t>
+          <t>223.35</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>45055</v>
+        <v>45050</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>21.30</t>
+          <t>220.95</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>45056</v>
+        <v>45051</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>21.27</t>
+          <t>215.95</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>45057</v>
+        <v>45054</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>21.26</t>
+          <t>217.00</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>45058</v>
+        <v>45055</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>21.70</t>
+          <t>215.90</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>45061</v>
+        <v>45056</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>21.88</t>
+          <t>212.35</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>45062</v>
+        <v>45057</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>21.98</t>
+          <t>211.60</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>45063</v>
+        <v>45058</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>21.86</t>
+          <t>212.00</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
-        <v>45064</v>
+        <v>45061</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>21.85</t>
+          <t>210.55</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
-        <v>45065</v>
+        <v>45062</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>21.83</t>
+          <t>209.05</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
-        <v>45069</v>
+        <v>45063</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>21.84</t>
+          <t>208.90</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
-        <v>45070</v>
+        <v>45064</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>21.70</t>
+          <t>210.05</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
-        <v>45071</v>
+        <v>45065</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>21.16</t>
+          <t>212.25</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
-        <v>45072</v>
+        <v>45068</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>21.15</t>
+          <t>211.60</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
-        <v>45075</v>
+        <v>45069</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>21.01</t>
+          <t>211.60</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
-        <v>45076</v>
+        <v>45070</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>20.94</t>
+          <t>205.90</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="n">
-        <v>45077</v>
+        <v>45071</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>20.80</t>
+          <t>205.60</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="n">
-        <v>45079</v>
+        <v>45072</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>19.83</t>
+          <t>207.40</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="n">
-        <v>45082</v>
+        <v>45075</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>19.52</t>
+          <t>207.75</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="n">
-        <v>45083</v>
+        <v>45076</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>19.27</t>
+          <t>207.35</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="n">
-        <v>45084</v>
+        <v>45077</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>19.01</t>
+          <t>199.98</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="n">
-        <v>45085</v>
+        <v>45078</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>18.82</t>
+          <t>204.20</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="2" t="n">
-        <v>45086</v>
+        <v>45079</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>18.86</t>
+          <t>210.15</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="2" t="n">
-        <v>45089</v>
+        <v>45082</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>18.97</t>
+          <t>209.95</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="2" t="n">
-        <v>45090</v>
+        <v>45083</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>18.79</t>
+          <t>210.50</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="2" t="n">
-        <v>45091</v>
+        <v>45084</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>19.20</t>
+          <t>208.85</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="2" t="n">
-        <v>45092</v>
+        <v>45085</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>19.42</t>
+          <t>208.90</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="2" t="n">
-        <v>45093</v>
+        <v>45086</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>19.24</t>
+          <t>207.95</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="2" t="n">
-        <v>45096</v>
+        <v>45089</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>19.31</t>
+          <t>208.60</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="2" t="n">
-        <v>45097</v>
+        <v>45090</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>19.20</t>
+          <t>208.95</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="2" t="n">
-        <v>45098</v>
+        <v>45091</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>19.23</t>
+          <t>209.75</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="2" t="n">
-        <v>45099</v>
+        <v>45092</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>19.43</t>
+          <t>209.80</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="2" t="n">
-        <v>45100</v>
+        <v>45093</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>19.53</t>
+          <t>210.30</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="2" t="n">
-        <v>45103</v>
+        <v>45096</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>19.69</t>
+          <t>210.00</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="2" t="n">
-        <v>45104</v>
+        <v>45097</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>19.73</t>
+          <t>209.25</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="2" t="n">
-        <v>45105</v>
+        <v>45098</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>20.06</t>
+          <t>208.90</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="2" t="n">
-        <v>45106</v>
+        <v>45099</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>19.95</t>
+          <t>208.45</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="2" t="n">
-        <v>45107</v>
+        <v>45100</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>20.02</t>
+          <t>209.15</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="2" t="n">
-        <v>45110</v>
+        <v>45103</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>19.90</t>
+          <t>209.20</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="2" t="n">
-        <v>45111</v>
+        <v>45104</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>19.99</t>
+          <t>211.30</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="2" t="n">
-        <v>45112</v>
+        <v>45105</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>19.90</t>
+          <t>211.65</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="2" t="n">
-        <v>45113</v>
+        <v>45106</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>19.71</t>
+          <t>211.05</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="2" t="n">
-        <v>45114</v>
+        <v>45107</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>19.48</t>
+          <t>213.20</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="2" t="n">
-        <v>45117</v>
+        <v>45110</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>19.41</t>
+          <t>213.75</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="2" t="n">
-        <v>45118</v>
+        <v>45111</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>19.41</t>
+          <t>213.20</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="2" t="n">
-        <v>45119</v>
+        <v>45112</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>19.63</t>
+          <t>207.55</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="2" t="n">
-        <v>45120</v>
+        <v>45113</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>19.83</t>
+          <t>203.20</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="2" t="n">
-        <v>45121</v>
+        <v>45114</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>19.90</t>
+          <t>204.00</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="2" t="n">
-        <v>45124</v>
+        <v>45117</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>19.66</t>
+          <t>205.85</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="2" t="n">
-        <v>45125</v>
+        <v>45118</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>19.40</t>
+          <t>207.85</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="2" t="n">
-        <v>45126</v>
+        <v>45119</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>19.43</t>
+          <t>211.10</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="2" t="n">
-        <v>45127</v>
+        <v>45120</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>19.63</t>
+          <t>212.15</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="2" t="n">
-        <v>45131</v>
+        <v>45121</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>19.89</t>
+          <t>210.35</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="2" t="n">
-        <v>45132</v>
+        <v>45124</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>19.82</t>
+          <t>210.20</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="2" t="n">
-        <v>45133</v>
+        <v>45125</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>19.60</t>
+          <t>210.80</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="2" t="n">
-        <v>45134</v>
+        <v>45126</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>19.85</t>
+          <t>210.60</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="2" t="n">
-        <v>45135</v>
+        <v>45127</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>19.89</t>
+          <t>214.35</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="2" t="n">
-        <v>45138</v>
+        <v>45128</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>19.86</t>
+          <t>214.60</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="2" t="n">
-        <v>45139</v>
+        <v>45131</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>19.78</t>
+          <t>215.25</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="2" t="n">
-        <v>45140</v>
+        <v>45132</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>19.45</t>
+          <t>216.10</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="2" t="n">
-        <v>45141</v>
+        <v>45133</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>18.79</t>
+          <t>215.80</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="2" t="n">
-        <v>45142</v>
+        <v>45134</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>18.82</t>
+          <t>218.85</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="2" t="n">
-        <v>45145</v>
+        <v>45135</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>18.70</t>
+          <t>219.30</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="2" t="n">
-        <v>45146</v>
+        <v>45138</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>18.53</t>
+          <t>217.40</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="2" t="n">
-        <v>45147</v>
+        <v>45139</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>18.74</t>
+          <t>215.90</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="2" t="n">
-        <v>45148</v>
+        <v>45140</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>18.96</t>
+          <t>211.75</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="2" t="n">
-        <v>45149</v>
+        <v>45141</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>18.80</t>
+          <t>211.50</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="2" t="n">
-        <v>45152</v>
+        <v>45142</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>18.99</t>
+          <t>214.00</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="2" t="n">
-        <v>45154</v>
+        <v>45145</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>18.88</t>
+          <t>215.05</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="2" t="n">
-        <v>45155</v>
+        <v>45146</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>18.89</t>
+          <t>212.65</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="2" t="n">
-        <v>45159</v>
+        <v>45147</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>19.14</t>
+          <t>214.50</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="2" t="n">
-        <v>45160</v>
+        <v>45148</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>19.15</t>
+          <t>225.00</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="2" t="n">
-        <v>45161</v>
+        <v>45149</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>19.30</t>
+          <t>223.25</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="2" t="n">
-        <v>45162</v>
+        <v>45152</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>19.30</t>
+          <t>224.30</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="2" t="n">
-        <v>45163</v>
+        <v>45153</v>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>19.25</t>
+          <t>221.25</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="2" t="n">
-        <v>45166</v>
+        <v>45154</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>19.45</t>
+          <t>221.75</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="2" t="n">
-        <v>45167</v>
+        <v>45155</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>19.53</t>
+          <t>221.95</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="2" t="n">
-        <v>45168</v>
+        <v>45156</v>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>19.56</t>
+          <t>221.15</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="2" t="n">
-        <v>45169</v>
+        <v>45159</v>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>19.74</t>
+          <t>220.80</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="2" t="n">
-        <v>45170</v>
+        <v>45160</v>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>19.80</t>
+          <t>221.10</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="2" t="n">
-        <v>45173</v>
+        <v>45161</v>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>19.61</t>
+          <t>221.75</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="2" t="n">
-        <v>45174</v>
+        <v>45162</v>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>19.81</t>
+          <t>222.40</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="2" t="n">
-        <v>45175</v>
+        <v>45163</v>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>19.94</t>
+          <t>222.10</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="2" t="n">
-        <v>45176</v>
+        <v>45166</v>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>20.05</t>
+          <t>224.70</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="2" t="n">
-        <v>45177</v>
+        <v>45167</v>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>20.07</t>
+          <t>225.50</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="2" t="n">
-        <v>45180</v>
+        <v>45168</v>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>20.45</t>
+          <t>225.10</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="2" t="n">
-        <v>45181</v>
+        <v>45169</v>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>20.57</t>
+          <t>224.35</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="2" t="n">
-        <v>45182</v>
+        <v>45170</v>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>20.56</t>
+          <t>224.25</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="2" t="n">
-        <v>45183</v>
+        <v>45173</v>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>20.70</t>
+          <t>223.30</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="2" t="n">
-        <v>45184</v>
+        <v>45174</v>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>20.65</t>
+          <t>221.95</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="2" t="n">
-        <v>45187</v>
+        <v>45175</v>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>20.56</t>
+          <t>221.25</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="2" t="n">
-        <v>45188</v>
+        <v>45176</v>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>20.59</t>
+          <t>221.25</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="2" t="n">
-        <v>45189</v>
+        <v>45177</v>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>20.70</t>
+          <t>222.25</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="2" t="n">
-        <v>45190</v>
+        <v>45180</v>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>20.52</t>
+          <t>224.75</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="2" t="n">
-        <v>45191</v>
+        <v>45181</v>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>20.56</t>
+          <t>226.80</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="2" t="n">
-        <v>45194</v>
+        <v>45182</v>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>20.05</t>
+          <t>227.35</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="2" t="n">
-        <v>45195</v>
+        <v>45183</v>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>20.00</t>
+          <t>231.50</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="2" t="n">
-        <v>45196</v>
+        <v>45184</v>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>19.67</t>
+          <t>233.45</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="2" t="n">
-        <v>45197</v>
+        <v>45187</v>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>19.79</t>
+          <t>231.50</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="2" t="n">
-        <v>45198</v>
+        <v>45188</v>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>19.98</t>
+          <t>233.35</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="2" t="n">
-        <v>45201</v>
+        <v>45189</v>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>19.96</t>
+          <t>231.40</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="2" t="n">
-        <v>45202</v>
+        <v>45190</v>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>19.78</t>
+          <t>229.95</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="2" t="n">
-        <v>45203</v>
+        <v>45191</v>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>19.76</t>
+          <t>232.15</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="2" t="n">
-        <v>45205</v>
+        <v>45194</v>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>19.95</t>
+          <t>229.35</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="2" t="n">
-        <v>45208</v>
+        <v>45195</v>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>20.27</t>
+          <t>230.45</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="2" t="n">
-        <v>45209</v>
+        <v>45196</v>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>20.46</t>
+          <t>226.95</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="2" t="n">
-        <v>45210</v>
+        <v>45197</v>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>20.61</t>
+          <t>228.55</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="2" t="n">
-        <v>45211</v>
+        <v>45198</v>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>20.56</t>
+          <t>225.70</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="2" t="n">
-        <v>45216</v>
+        <v>45201</v>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>20.30</t>
+          <t>222.70</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="2" t="n">
-        <v>45217</v>
+        <v>45202</v>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>20.42</t>
+          <t>220.95</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="2" t="n">
-        <v>45218</v>
+        <v>45203</v>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>20.27</t>
+          <t>219.65</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="2" t="n">
-        <v>45219</v>
+        <v>45204</v>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>20.15</t>
+          <t>220.70</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="2" t="n">
-        <v>45222</v>
+        <v>45205</v>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>20.06</t>
+          <t>224.30</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="2" t="n">
-        <v>45223</v>
+        <v>45208</v>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>20.17</t>
+          <t>222.50</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="2" t="n">
-        <v>45224</v>
+        <v>45209</v>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>20.38</t>
+          <t>225.25</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="2" t="n">
-        <v>45225</v>
+        <v>45210</v>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>20.42</t>
+          <t>226.95</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="2" t="n">
-        <v>45226</v>
+        <v>45211</v>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>20.52</t>
+          <t>226.50</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="2" t="n">
-        <v>45229</v>
+        <v>45212</v>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>20.43</t>
+          <t>222.80</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="2" t="n">
-        <v>45230</v>
+        <v>45215</v>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>20.49</t>
+          <t>224.25</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="2" t="n">
-        <v>45232</v>
+        <v>45216</v>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>21.35</t>
+          <t>224.55</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="2" t="n">
-        <v>45233</v>
+        <v>45217</v>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>21.32</t>
+          <t>223.30</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="2" t="n">
-        <v>45236</v>
+        <v>45218</v>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>21.55</t>
+          <t>221.25</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="2" t="n">
-        <v>45237</v>
+        <v>45219</v>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>21.30</t>
+          <t>217.40</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="2" t="n">
-        <v>45238</v>
+        <v>45222</v>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>21.13</t>
+          <t>217.80</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="2" t="n">
-        <v>45239</v>
+        <v>45223</v>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>21.53</t>
+          <t>218.15</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="2" t="n">
-        <v>45240</v>
+        <v>45224</v>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>22.19</t>
+          <t>220.15</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="2" t="n">
-        <v>45243</v>
+        <v>45225</v>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>21.53</t>
+          <t>219.55</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="2" t="n">
-        <v>45244</v>
+        <v>45226</v>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>21.55</t>
+          <t>218.60</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="2" t="n">
-        <v>45245</v>
+        <v>45229</v>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>21.32</t>
+          <t>221.05</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="2" t="n">
-        <v>45246</v>
+        <v>45230</v>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>21.37</t>
+          <t>220.90</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="2" t="n">
-        <v>45247</v>
+        <v>45231</v>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>21.43</t>
+          <t>224.25</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="2" t="n">
-        <v>45250</v>
+        <v>45232</v>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>21.58</t>
+          <t>223.60</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="2" t="n">
-        <v>45251</v>
+        <v>45233</v>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>21.36</t>
+          <t>221.00</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="2" t="n">
-        <v>45252</v>
+        <v>45236</v>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>21.73</t>
+          <t>221.15</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="2" t="n">
-        <v>45253</v>
+        <v>45237</v>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>21.70</t>
+          <t>218.85</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="2" t="n">
-        <v>45254</v>
+        <v>45238</v>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>21.87</t>
+          <t>220.75</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="2" t="n">
-        <v>45257</v>
+        <v>45239</v>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>22.05</t>
+          <t>222.30</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="2" t="n">
-        <v>45258</v>
+        <v>45240</v>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>21.86</t>
+          <t>222.00</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="2" t="n">
-        <v>45259</v>
+        <v>45243</v>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>21.88</t>
+          <t>221.40</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="2" t="n">
-        <v>45260</v>
+        <v>45244</v>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>21.88</t>
+          <t>224.50</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="2" t="n">
-        <v>45261</v>
+        <v>45245</v>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>22.07</t>
+          <t>224.50</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="2" t="n">
-        <v>45264</v>
+        <v>45246</v>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>22.43</t>
+          <t>226.15</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="2" t="n">
-        <v>45265</v>
+        <v>45247</v>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>22.55</t>
+          <t>228.50</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="2" t="n">
-        <v>45266</v>
+        <v>45250</v>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>22.63</t>
+          <t>228.80</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="2" t="n">
-        <v>45267</v>
+        <v>45251</v>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>22.59</t>
+          <t>230.35</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="2" t="n">
-        <v>45268</v>
+        <v>45252</v>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>22.63</t>
+          <t>231.00</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="2" t="n">
-        <v>45271</v>
+        <v>45253</v>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>22.85</t>
+          <t>232.30</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="2" t="n">
-        <v>45272</v>
+        <v>45254</v>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>22.79</t>
+          <t>232.70</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="2" t="n">
-        <v>45273</v>
+        <v>45257</v>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>22.54</t>
+          <t>230.50</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="2" t="n">
-        <v>45274</v>
+        <v>45258</v>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>21.77</t>
+          <t>230.55</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="2" t="n">
-        <v>45275</v>
+        <v>45259</v>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>21.60</t>
+          <t>231.00</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="2" t="n">
-        <v>45278</v>
+        <v>45260</v>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>21.50</t>
+          <t>230.60</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="2" t="n">
-        <v>45279</v>
+        <v>45261</v>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>21.44</t>
+          <t>235.25</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="2" t="n">
-        <v>45280</v>
+        <v>45264</v>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>21.52</t>
+          <t>235.10</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="2" t="n">
-        <v>45281</v>
+        <v>45265</v>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>21.65</t>
+          <t>238.75</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="2" t="n">
-        <v>45282</v>
+        <v>45266</v>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>21.78</t>
+          <t>240.95</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="2" t="n">
-        <v>45287</v>
+        <v>45267</v>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>21.65</t>
+          <t>242.15</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="2" t="n">
-        <v>45288</v>
+        <v>45268</v>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>21.60</t>
+          <t>243.80</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="2" t="n">
-        <v>45289</v>
+        <v>45271</v>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>21.61</t>
+          <t>245.40</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="2" t="n">
-        <v>45293</v>
+        <v>45272</v>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>21.97</t>
+          <t>245.50</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="2" t="n">
-        <v>45294</v>
+        <v>45273</v>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>22.28</t>
+          <t>244.95</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="2" t="n">
-        <v>45295</v>
+        <v>45274</v>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>22.43</t>
+          <t>239.00</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="2" t="n">
-        <v>45296</v>
+        <v>45275</v>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>22.48</t>
+          <t>240.20</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="2" t="n">
-        <v>45299</v>
+        <v>45278</v>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>22.51</t>
+          <t>240.70</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="2" t="n">
-        <v>45300</v>
+        <v>45279</v>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>22.48</t>
+          <t>242.50</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="2" t="n">
-        <v>45301</v>
+        <v>45280</v>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>22.50</t>
+          <t>242.25</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="2" t="n">
-        <v>45302</v>
+        <v>45281</v>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>22.33</t>
+          <t>241.65</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="2" t="n">
-        <v>45303</v>
+        <v>45282</v>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>22.48</t>
+          <t>242.60</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="2" t="n">
-        <v>45306</v>
+        <v>45287</v>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>22.50</t>
+          <t>241.70</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="2" t="n">
-        <v>45307</v>
+        <v>45288</v>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>22.76</t>
+          <t>240.65</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="2" t="n">
-        <v>45308</v>
+        <v>45289</v>
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>22.72</t>
+          <t>241.95</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="2" t="n">
-        <v>45309</v>
+        <v>45293</v>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>22.83</t>
+          <t>244.95</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="2" t="n">
-        <v>45310</v>
+        <v>45294</v>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>23.03</t>
+          <t>242.55</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" s="2" t="n">
-        <v>45313</v>
+        <v>45295</v>
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>23.27</t>
+          <t>245.50</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" s="2" t="n">
-        <v>45314</v>
+        <v>45296</v>
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>23.26</t>
+          <t>243.90</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" s="2" t="n">
-        <v>45315</v>
+        <v>45299</v>
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>23.31</t>
+          <t>244.55</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" s="2" t="n">
-        <v>45316</v>
+        <v>45300</v>
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>23.24</t>
+          <t>243.55</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="2" t="n">
-        <v>45317</v>
+        <v>45301</v>
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>23.07</t>
+          <t>242.20</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" s="2" t="n">
-        <v>45320</v>
+        <v>45302</v>
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>22.97</t>
+          <t>239.65</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="2" t="n">
-        <v>45321</v>
+        <v>45303</v>
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>22.91</t>
+          <t>241.70</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="2" t="n">
-        <v>45322</v>
+        <v>45306</v>
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>22.73</t>
+          <t>241.80</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="2" t="n">
-        <v>45323</v>
+        <v>45307</v>
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>22.72</t>
+          <t>242.65</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="2" t="n">
-        <v>45324</v>
+        <v>45308</v>
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>22.64</t>
+          <t>244.85</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="2" t="n">
-        <v>45327</v>
+        <v>45309</v>
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>22.62</t>
+          <t>245.35</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="2" t="n">
-        <v>45328</v>
+        <v>45310</v>
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>22.66</t>
+          <t>247.15</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="2" t="n">
-        <v>45329</v>
+        <v>45313</v>
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>22.38</t>
+          <t>249.85</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="2" t="n">
-        <v>45330</v>
+        <v>45314</v>
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>22.13</t>
+          <t>245.40</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="2" t="n">
-        <v>45331</v>
+        <v>45315</v>
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>22.17</t>
+          <t>248.50</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="2" t="n">
-        <v>45334</v>
+        <v>45316</v>
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>22.25</t>
+          <t>246.85</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="2" t="n">
-        <v>45335</v>
+        <v>45317</v>
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>22.23</t>
+          <t>248.10</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="2" t="n">
-        <v>45336</v>
+        <v>45320</v>
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>22.08</t>
+          <t>246.55</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="2" t="n">
-        <v>45337</v>
+        <v>45321</v>
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>22.11</t>
+          <t>247.60</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="2" t="n">
-        <v>45338</v>
+        <v>45322</v>
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>22.14</t>
+          <t>247.80</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="2" t="n">
-        <v>45341</v>
+        <v>45323</v>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>22.31</t>
+          <t>245.25</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="2" t="n">
-        <v>45342</v>
+        <v>45324</v>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>22.26</t>
+          <t>245.90</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="2" t="n">
-        <v>45343</v>
+        <v>45327</v>
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>22.20</t>
+          <t>245.40</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="2" t="n">
-        <v>45344</v>
+        <v>45328</v>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>22.33</t>
+          <t>248.10</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="2" t="n">
-        <v>45345</v>
+        <v>45329</v>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>22.17</t>
+          <t>245.25</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="2" t="n">
-        <v>45348</v>
+        <v>45330</v>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>22.00</t>
+          <t>243.85</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="2" t="n">
-        <v>45349</v>
+        <v>45331</v>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>22.08</t>
+          <t>243.00</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="2" t="n">
-        <v>45350</v>
+        <v>45334</v>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>21.99</t>
+          <t>246.25</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="2" t="n">
-        <v>45351</v>
+        <v>45335</v>
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>22.01</t>
+          <t>245.70</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="2" t="n">
-        <v>45352</v>
+        <v>45336</v>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>21.97</t>
+          <t>244.60</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="2" t="n">
-        <v>45355</v>
+        <v>45337</v>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>21.97</t>
+          <t>246.00</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="2" t="n">
-        <v>45356</v>
+        <v>45338</v>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>22.22</t>
+          <t>247.10</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="2" t="n">
-        <v>45357</v>
+        <v>45341</v>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>22.26</t>
+          <t>248.65</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="2" t="n">
-        <v>45358</v>
+        <v>45342</v>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>22.14</t>
+          <t>249.40</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="2" t="n">
-        <v>45359</v>
+        <v>45343</v>
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>21.89</t>
+          <t>250.70</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="2" t="n">
-        <v>45362</v>
+        <v>45344</v>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>21.84</t>
+          <t>255.10</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="2" t="n">
-        <v>45363</v>
+        <v>45345</v>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>21.76</t>
+          <t>246.50</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="2" t="n">
-        <v>45364</v>
+        <v>45348</v>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>21.59</t>
+          <t>245.65</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="2" t="n">
-        <v>45365</v>
+        <v>45349</v>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>21.55</t>
+          <t>248.00</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="2" t="n">
-        <v>45366</v>
+        <v>45350</v>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>21.80</t>
+          <t>248.55</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="2" t="n">
-        <v>45369</v>
+        <v>45351</v>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>21.69</t>
+          <t>253.85</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="2" t="n">
-        <v>45370</v>
+        <v>45352</v>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>21.91</t>
+          <t>251.80</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="2" t="n">
-        <v>45371</v>
+        <v>45355</v>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>21.89</t>
+          <t>252.00</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="2" t="n">
-        <v>45372</v>
+        <v>45356</v>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>21.91</t>
+          <t>254.45</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="2" t="n">
-        <v>45373</v>
+        <v>45357</v>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>21.80</t>
+          <t>254.60</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="2" t="n">
-        <v>45376</v>
+        <v>45358</v>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>21.76</t>
+          <t>256.30</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="2" t="n">
-        <v>45377</v>
+        <v>45359</v>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>22.49</t>
+          <t>258.80</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="2" t="n">
-        <v>45378</v>
+        <v>45362</v>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>22.45</t>
+          <t>260.25</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="2" t="n">
-        <v>45379</v>
+        <v>45363</v>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>22.46</t>
+          <t>263.85</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="2" t="n">
-        <v>45384</v>
+        <v>45364</v>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>22.38</t>
+          <t>265.45</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="2" t="n">
-        <v>45385</v>
+        <v>45365</v>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>22.23</t>
+          <t>264.60</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="2" t="n">
-        <v>45386</v>
+        <v>45366</v>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>22.25</t>
+          <t>266.65</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="2" t="n">
+        <v>45369</v>
+      </c>
+      <c r="B246" t="inlineStr">
+        <is>
+          <t>266.20</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" s="2" t="n">
+        <v>45370</v>
+      </c>
+      <c r="B247" t="inlineStr">
+        <is>
+          <t>271.05</t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" s="2" t="n">
+        <v>45371</v>
+      </c>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t>271.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" s="2" t="n">
+        <v>45372</v>
+      </c>
+      <c r="B249" t="inlineStr">
+        <is>
+          <t>272.90</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" s="2" t="n">
+        <v>45373</v>
+      </c>
+      <c r="B250" t="inlineStr">
+        <is>
+          <t>271.85</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" s="2" t="n">
+        <v>45376</v>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>275.20</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" s="2" t="n">
+        <v>45377</v>
+      </c>
+      <c r="B252" t="inlineStr">
+        <is>
+          <t>277.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" s="2" t="n">
+        <v>45378</v>
+      </c>
+      <c r="B253" t="inlineStr">
+        <is>
+          <t>277.45</t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" s="2" t="n">
+        <v>45379</v>
+      </c>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t>277.80</t>
+        </is>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" s="2" t="n">
+        <v>45384</v>
+      </c>
+      <c r="B255" t="inlineStr">
+        <is>
+          <t>273.90</t>
+        </is>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" s="2" t="n">
+        <v>45385</v>
+      </c>
+      <c r="B256" t="inlineStr">
+        <is>
+          <t>274.40</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" s="2" t="n">
+        <v>45386</v>
+      </c>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t>272.40</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" s="2" t="n">
         <v>45387</v>
       </c>
-      <c r="B246" t="inlineStr">
-        <is>
-          <t>21.88</t>
+      <c r="B258" t="inlineStr">
+        <is>
+          <t>268.80</t>
         </is>
       </c>
     </row>

</xml_diff>